<commit_message>
AntrProyecto.. continua plan de proyecto.. documentación de EncuestaUsuarios1
</commit_message>
<xml_diff>
--- a/Documentacion/HorasFede.xlsx
+++ b/Documentacion/HorasFede.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="19">
   <si>
     <t>Horas trabajadas</t>
   </si>
@@ -75,6 +75,12 @@
   </si>
   <si>
     <t>Plan de proyecto, Metodologías, Cilco de vida, incremento o itereaciones definidas, integrantes y roles, descripción y selección de herramientas</t>
+  </si>
+  <si>
+    <t>Plan de SQA, estandares definidos y convenciones</t>
+  </si>
+  <si>
+    <t>Plan de testing, Pland de SCM, Plan de capacitación. Documentación de EncuestaUsuarios1</t>
   </si>
 </sst>
 </file>
@@ -393,10 +399,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -552,6 +558,9 @@
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>4</v>
+      </c>
       <c r="B10" s="1">
         <v>42835</v>
       </c>
@@ -566,6 +575,9 @@
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>4</v>
+      </c>
       <c r="B11" s="1">
         <v>42835</v>
       </c>
@@ -580,6 +592,9 @@
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>4</v>
+      </c>
       <c r="B12" s="1">
         <v>42836</v>
       </c>
@@ -591,6 +606,37 @@
       </c>
       <c r="E12" t="s">
         <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>4</v>
+      </c>
+      <c r="B13" s="1">
+        <v>42837</v>
+      </c>
+      <c r="C13">
+        <v>2</v>
+      </c>
+      <c r="D13" t="s">
+        <v>6</v>
+      </c>
+      <c r="E13" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B14" s="1">
+        <v>42838</v>
+      </c>
+      <c r="C14">
+        <v>3</v>
+      </c>
+      <c r="D14" t="s">
+        <v>6</v>
+      </c>
+      <c r="E14" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>